<commit_message>
importação empresa - 2
segue a importação da empresa - 2
</commit_message>
<xml_diff>
--- a/Nova Planilha DP.xlsx
+++ b/Nova Planilha DP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Micro\Documents\GitHub\intelig-ncia-de-dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF7B36EE-C15B-44B7-BC9D-CCF40EA07BED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F547BCF5-DB0D-49C1-9046-1639C532DAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{3021E2C6-A2FA-449C-AA56-3B5F4B755610}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
   <si>
     <t>COLABORADOR</t>
   </si>
@@ -45,6 +45,21 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>53:17</t>
+  </si>
+  <si>
+    <t>07:07</t>
+  </si>
+  <si>
+    <t>97:52</t>
+  </si>
+  <si>
+    <t>60:20</t>
+  </si>
+  <si>
+    <t>218:38</t>
   </si>
 </sst>
 </file>
@@ -417,7 +432,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -558,6 +573,21 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -629,7 +659,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -643,15 +673,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="46" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="46" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="63">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1028,10 +1053,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD5F1B4F-51F2-48B8-A03E-24D62E83EFA1}">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1040,10 +1065,9 @@
     <col min="2" max="2" width="12" style="1" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1051,139 +1075,129 @@
         <v>1</v>
       </c>
       <c r="C1" s="4">
+        <v>395</v>
+      </c>
+      <c r="D1" s="4">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="6">
+        <v>123</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="6"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="6">
+        <v>130</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4">
-        <v>957</v>
-      </c>
-      <c r="E1" s="4">
-        <v>64</v>
-      </c>
-      <c r="F1" s="4">
-        <v>3</v>
-      </c>
-      <c r="G1" s="4">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="6">
-        <v>41</v>
-      </c>
-      <c r="C2" s="5">
-        <v>5.3520833333333337</v>
-      </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5">
-        <v>1.2222222222222223</v>
-      </c>
-      <c r="F2" s="5">
-        <v>1.8333333333333333</v>
-      </c>
-      <c r="G2" s="6">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="6">
-        <v>37</v>
-      </c>
-      <c r="C3" s="5">
-        <v>7.6062500000000002</v>
-      </c>
-      <c r="D3" s="5">
-        <v>3.0555555555555555E-2</v>
-      </c>
-      <c r="E3" s="5">
-        <v>0.30555555555555558</v>
-      </c>
-      <c r="F3" s="5">
-        <v>1.5277777777777777</v>
-      </c>
-      <c r="G3" s="6">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D3" s="6">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" s="6">
-        <v>39</v>
-      </c>
-      <c r="C4" s="5">
-        <v>7.9625000000000004</v>
-      </c>
-      <c r="D4" s="5">
-        <v>6.458333333333334E-2</v>
-      </c>
-      <c r="E4" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="5">
-        <v>1.2222222222222223</v>
-      </c>
-      <c r="G4" s="6">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D4" s="6">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" s="6">
-        <v>36</v>
-      </c>
-      <c r="C5" s="5">
-        <v>6.6881944444444441</v>
-      </c>
-      <c r="D5" s="5">
-        <v>7.4305555555555555E-2</v>
-      </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5">
-        <v>1.5277777777777777</v>
-      </c>
-      <c r="G5" s="6">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="6">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="6">
-        <v>32</v>
-      </c>
-      <c r="C6" s="5">
-        <v>7.6624999999999996</v>
-      </c>
-      <c r="D6" s="5">
-        <v>0.14166666666666666</v>
-      </c>
-      <c r="E6" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="6">
+        <v>118</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="6"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="6">
+        <v>78</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="5">
-        <v>1.5277777777777777</v>
-      </c>
-      <c r="G6" s="6">
-        <v>600</v>
-      </c>
-      <c r="L6" s="8"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C10" s="9"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G15" s="7"/>
+      <c r="D8" s="6">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="6">
+        <v>135</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="6">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="6">
+        <v>117</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="6"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="6">
+        <v>126</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="6">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="6"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:B1" xr:uid="{FD5F1B4F-51F2-48B8-A03E-24D62E83EFA1}"/>

</xml_diff>